<commit_message>
data abicare excel files.
</commit_message>
<xml_diff>
--- a/code/screpo/data/abicare/exmileageMonmouthshire08Nov.xlsx
+++ b/code/screpo/data/abicare/exmileageMonmouthshire08Nov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah4c20\Asyl\PostDoc\SOCIALCARE\code\screpo\data\abicare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF91A3F3-03A1-4524-9B1B-236A7F3FDE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2660D9FC-192F-49E5-84E6-1410BEBA719B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1275,7 +1275,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>